<commit_message>
Se modifica diagrama de rendimiento
</commit_message>
<xml_diff>
--- a/Analisis de rendimiento.xlsx
+++ b/Analisis de rendimiento.xlsx
@@ -171,21 +171,33 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Análisis de Rendimiento</a:t>
+              <a:rPr lang="es-AR"/>
+              <a:t>Análisis</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" baseline="0"/>
+              <a:t> de Rendimiento</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -203,12 +215,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -221,56 +240,579 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Msucesivas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1122.164</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1513.896</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1959.511</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1331.2860000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1676.8309999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2454.306</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Recursiva</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>105.63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71.418000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.215000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>161.226</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>361.79500000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>883.53300000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RecursivaPar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53.884999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.147999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.838999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>194.583</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>336.56400000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ProgDinamica</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mejorada</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
             </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
-            <c:spPr>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </c:spPr>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -286,36 +828,40 @@
                 <c:pt idx="4">
                   <c:v>100</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>Sheet1!$H$2:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>43.621000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>83.82</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>56.451000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>75.268000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78.260000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>153.566</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1839-4621-9264-A8B8E811C78A}"/>
-            </c:ext>
-          </c:extLst>
+          </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -325,31 +871,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="332013896"/>
-        <c:axId val="332012720"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="332013896"/>
+        <c:smooth val="0"/>
+        <c:axId val="368926096"/>
+        <c:axId val="368925312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="368926096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -357,10 +889,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                        <a:lumMod val="85000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -369,9 +901,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Grado</a:t>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>GRADO</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="es-AR" baseline="0"/>
+                  <a:t> DEL POLINOMIO</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-AR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -389,121 +926,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:noFill/>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="332012720"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="332012720"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Tiempo (milisegundos)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                      <a:lumMod val="85000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -524,7 +950,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -539,7 +966,7 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -550,9 +977,127 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332013896"/>
+        <c:crossAx val="368925312"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="368925312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>TIEMPO (MICROSEGUNDOS)</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="368926096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -562,25 +1107,64 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -643,17 +1227,17 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -661,36 +1245,52 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -698,7 +1298,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -708,17 +1308,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="15000"/>
-        <a:lumOff val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -727,131 +1324,72 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
-      <a:effectLst>
-        <a:glow rad="139700">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="14000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:lumMod val="60000"/>
-          <a:lumOff val="40000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -868,15 +1406,15 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -888,22 +1426,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -912,16 +1450,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -930,13 +1469,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -948,7 +1487,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -961,10 +1500,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -979,90 +1517,100 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1070,13 +1618,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1089,10 +1638,18 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1101,14 +1658,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="25400" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -1119,7 +1674,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1129,21 +1684,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1153,28 +1706,17 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -1184,26 +1726,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>356234</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C74A11AD-B747-4EA5-960D-9F6D0927FA16}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1521,7 +2057,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1565,19 +2101,25 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
+        <v>1122.164</v>
+      </c>
+      <c r="C2" s="1">
+        <v>105.63</v>
+      </c>
+      <c r="D2" s="1">
+        <v>53.884999999999998</v>
+      </c>
+      <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>43.621000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1585,19 +2127,25 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
+        <v>1513.896</v>
+      </c>
+      <c r="C3" s="1">
+        <v>71.418000000000006</v>
+      </c>
+      <c r="D3" s="1">
+        <v>91.09</v>
+      </c>
+      <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="D3" s="1">
+      <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>83.82</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1605,19 +2153,25 @@
         <v>20</v>
       </c>
       <c r="B4" s="1">
+        <v>1959.511</v>
+      </c>
+      <c r="C4" s="1">
+        <v>99.215000000000003</v>
+      </c>
+      <c r="D4" s="1">
+        <v>64.147999999999996</v>
+      </c>
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="1">
+      <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>56.451000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1625,42 +2179,78 @@
         <v>50</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1331.2860000000001</v>
       </c>
       <c r="C5" s="1">
+        <v>161.226</v>
+      </c>
+      <c r="D5" s="1">
+        <v>74.838999999999999</v>
+      </c>
+      <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="1">
+      <c r="F5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>75.268000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>100</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="B6" s="1">
+        <v>1676.8309999999999</v>
+      </c>
+      <c r="C6" s="1">
+        <v>361.79500000000002</v>
+      </c>
+      <c r="D6" s="1">
+        <v>194.583</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>78.260000000000005</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="A7" s="1">
+        <v>300</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2454.306</v>
+      </c>
+      <c r="C7" s="1">
+        <v>883.53300000000002</v>
+      </c>
+      <c r="D7" s="1">
+        <v>336.56400000000002</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>153.566</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>

</xml_diff>